<commit_message>
Comit start of justiyfy the variabels
</commit_message>
<xml_diff>
--- a/Data/Labour force by NUTS2.xlsx
+++ b/Data/Labour force by NUTS2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ha_b_\OneDrive\Documents\Skole\Assignments_MSB104\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF8F16-855B-4443-867F-134C177D0908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D6C846-C017-497C-8B1D-09C7CC3BEDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="130">
   <si>
     <t>Data extracted on 08/11/2025 01:27:24 from [ESTAT]</t>
   </si>
@@ -40,31 +40,16 @@
     <t>Time frequency [FREQ]</t>
   </si>
   <si>
-    <t>Annual [A]</t>
-  </si>
-  <si>
     <t>Unit of measure [UNIT]</t>
   </si>
   <si>
-    <t>Thousand persons [THS_PER]</t>
-  </si>
-  <si>
     <t>Sex [SEX]</t>
   </si>
   <si>
-    <t>Total [T]</t>
-  </si>
-  <si>
     <t>Age class [AGE]</t>
   </si>
   <si>
-    <t>15 years or over [Y_GE15]</t>
-  </si>
-  <si>
     <t>TIME</t>
-  </si>
-  <si>
-    <t>2016</t>
   </si>
   <si>
     <t/>
@@ -892,28 +877,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="11" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -921,7 +906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -929,862 +914,679 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C13" s="9">
+        <v>1495.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C14" s="12">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="10">
-        <v>2253.4</v>
-      </c>
-      <c r="D12" s="12">
-        <v>2274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C15" s="9">
+        <v>1021.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="9">
-        <v>1471.3</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1495.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C16" s="10">
+        <v>2614.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="10">
-        <v>1227.2</v>
-      </c>
-      <c r="D14" s="12">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C17" s="9">
+        <v>676.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="9">
-        <v>1013.1</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1021.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C18" s="10">
+        <v>598.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="10">
-        <v>2582.1</v>
-      </c>
-      <c r="D16" s="10">
-        <v>2614.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C19" s="9">
+        <v>574.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="9">
-        <v>667.4</v>
-      </c>
-      <c r="D17" s="9">
-        <v>676.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C20" s="10">
+        <v>937.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="10">
-        <v>591.9</v>
-      </c>
-      <c r="D18" s="10">
-        <v>598.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C21" s="9">
+        <v>704.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="11">
-        <v>580</v>
-      </c>
-      <c r="D19" s="9">
-        <v>574.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C22" s="10">
+        <v>1020.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="10">
-        <v>932.7</v>
-      </c>
-      <c r="D20" s="10">
-        <v>937.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C23" s="11">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="9">
-        <v>699.7</v>
-      </c>
-      <c r="D21" s="9">
-        <v>704.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C24" s="10">
+        <v>1298.5999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="10">
-        <v>1005.3</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1020.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C25" s="9">
+        <v>340.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="9">
-        <v>1885.3</v>
-      </c>
-      <c r="D23" s="11">
-        <v>1926</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C26" s="12">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="10">
-        <v>1307.2</v>
-      </c>
-      <c r="D24" s="10">
-        <v>1298.5999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C27" s="9">
+        <v>2100.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="9">
-        <v>344.5</v>
-      </c>
-      <c r="D25" s="9">
-        <v>340.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C28" s="12">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="10">
-        <v>979.5</v>
-      </c>
-      <c r="D26" s="12">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C29" s="9">
+        <v>626.79999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="9">
-        <v>2080.1</v>
-      </c>
-      <c r="D27" s="9">
-        <v>2100.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C30" s="10">
+        <v>797.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="10">
-        <v>550.9</v>
-      </c>
-      <c r="D28" s="12">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C31" s="11">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="9">
-        <v>615.20000000000005</v>
-      </c>
-      <c r="D29" s="9">
-        <v>626.79999999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C32" s="10">
+        <v>1090.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="10">
-        <v>809.3</v>
-      </c>
-      <c r="D30" s="10">
-        <v>797.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C33" s="11">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="11">
-        <v>799</v>
-      </c>
-      <c r="D31" s="11">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C34" s="10">
+        <v>1321.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="10">
-        <v>1078.7</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1090.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C35" s="9">
+        <v>2613.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="9">
-        <v>867.3</v>
-      </c>
-      <c r="D33" s="11">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C36" s="10">
+        <v>2274.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="12">
-        <v>1315</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1321.7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C37" s="9">
+        <v>1316.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="9">
-        <v>2566.6</v>
-      </c>
-      <c r="D35" s="9">
-        <v>2613.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C38" s="10">
+        <v>1050.5999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="12">
-        <v>2273</v>
-      </c>
-      <c r="D36" s="10">
-        <v>2274.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C39" s="9">
+        <v>1774.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="9">
-        <v>1317.1</v>
-      </c>
-      <c r="D37" s="9">
-        <v>1316.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C40" s="10">
+        <v>776.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="10">
-        <v>1060.4000000000001</v>
-      </c>
-      <c r="D38" s="10">
-        <v>1050.5999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C41" s="9">
+        <v>291.10000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="9">
-        <v>1776.5</v>
-      </c>
-      <c r="D39" s="9">
-        <v>1774.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C42" s="10">
+        <v>1063.4000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="10">
-        <v>777.3</v>
-      </c>
-      <c r="D40" s="10">
-        <v>776.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C43" s="9">
+        <v>500.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="9">
-        <v>288.89999999999998</v>
-      </c>
-      <c r="D41" s="9">
-        <v>291.10000000000002</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C44" s="10">
+        <v>808.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="10">
-        <v>1056.5</v>
-      </c>
-      <c r="D42" s="10">
-        <v>1063.4000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C45" s="9">
+        <v>728.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="11">
-        <v>504</v>
-      </c>
-      <c r="D43" s="9">
-        <v>500.7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C46" s="10">
+        <v>531.20000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="10">
-        <v>804.6</v>
-      </c>
-      <c r="D44" s="10">
-        <v>808.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C47" s="9">
+        <v>1104.0999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="9">
-        <v>735.6</v>
-      </c>
-      <c r="D45" s="9">
-        <v>728.6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C48" s="10">
+        <v>1468.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="10">
-        <v>542.4</v>
-      </c>
-      <c r="D46" s="10">
-        <v>531.20000000000005</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="C49" s="11">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="9">
-        <v>1126.2</v>
-      </c>
-      <c r="D47" s="9">
-        <v>1104.0999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C50" s="12">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="9">
+        <v>770.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="10">
+        <v>1176.9000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="9">
+        <v>442.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="10">
+        <v>572.79999999999995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="12">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="9">
+        <v>367.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="12">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="9">
+        <v>1083.9000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="10">
+        <v>662.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="9">
+        <v>896.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="10">
+        <v>693.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="9">
+        <v>480.4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="10">
+        <v>185.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="10">
-        <v>1445.3</v>
-      </c>
-      <c r="D48" s="10">
-        <v>1468.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="9">
-        <v>1108.5</v>
-      </c>
-      <c r="D49" s="11">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="10">
-        <v>401.5</v>
-      </c>
-      <c r="D50" s="12">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="9">
-        <v>766.8</v>
-      </c>
-      <c r="D51" s="9">
-        <v>770.9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="10">
-        <v>1158.7</v>
-      </c>
-      <c r="D52" s="10">
-        <v>1176.9000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="9">
-        <v>466.3</v>
-      </c>
-      <c r="D55" s="9">
-        <v>442.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="10">
-        <v>572.9</v>
-      </c>
-      <c r="D56" s="10">
-        <v>572.79999999999995</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="10">
-        <v>367.9</v>
-      </c>
-      <c r="D58" s="12">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="9">
-        <v>370.6</v>
-      </c>
-      <c r="D59" s="9">
-        <v>367.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" s="10">
-        <v>859.5</v>
-      </c>
-      <c r="D60" s="12">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" s="9">
-        <v>1073.5999999999999</v>
-      </c>
-      <c r="D61" s="9">
-        <v>1083.9000000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" s="10">
-        <v>660.9</v>
-      </c>
-      <c r="D62" s="10">
-        <v>662.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" s="9">
-        <v>888.8</v>
-      </c>
-      <c r="D63" s="9">
-        <v>896.6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="10">
-        <v>689.6</v>
-      </c>
-      <c r="D64" s="10">
-        <v>693.1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="9">
-        <v>485.4</v>
-      </c>
-      <c r="D65" s="9">
-        <v>480.4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
+      <c r="B71" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="10">
-        <v>184.2</v>
-      </c>
-      <c r="D66" s="10">
-        <v>185.2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>